<commit_message>
Logic to fire warm requests to target Lambdas
</commit_message>
<xml_diff>
--- a/lambda-startup-time-analysis.xlsx
+++ b/lambda-startup-time-analysis.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmbyr\Dropbox\Dashbird\xlambda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3119AE-5077-401A-8565-82055B5DBFC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518D81F7-C765-4BFB-AC4A-757775767674}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{112F00D6-EA6A-4222-B5E9-5C90DFE88A45}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{112F00D6-EA6A-4222-B5E9-5C90DFE88A45}"/>
   </bookViews>
   <sheets>
-    <sheet name="Stats" sheetId="1" r:id="rId1"/>
-    <sheet name="Regression - csharp" sheetId="7" r:id="rId2"/>
-    <sheet name="Regression - java" sheetId="6" r:id="rId3"/>
-    <sheet name="Regression - nodejs" sheetId="8" r:id="rId4"/>
-    <sheet name="Regression - python" sheetId="9" r:id="rId5"/>
+    <sheet name="Source" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="10" r:id="rId2"/>
+    <sheet name="Regression - csharp" sheetId="7" r:id="rId3"/>
+    <sheet name="Regression - java" sheetId="6" r:id="rId4"/>
+    <sheet name="Regression - nodejs" sheetId="8" r:id="rId5"/>
+    <sheet name="Regression - python" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Stats!$D$2</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Source!$D$2</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="41">
   <si>
     <t>csharp</t>
   </si>
@@ -231,12 +232,15 @@
       <t>: Yan Cui</t>
     </r>
   </si>
+  <si>
+    <t>X Variable</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +250,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -270,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +309,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,22 +351,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1622,37 +1641,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC1A1C7B-91B1-48F8-847F-64F1D24B3C20}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +1690,7 @@
         <v>8.5853713310993491</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1690,7 +1709,7 @@
         <v>8.0196456885960892</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1709,7 +1728,7 @@
         <v>7.5748767087176923</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1728,7 +1747,7 @@
         <v>7.1855233699201051</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -1747,102 +1766,102 @@
         <v>6.9560214963916254</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <v>128</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <v>5100.8900000000003</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="8">
         <f t="shared" si="0"/>
         <v>4.8520302639196169</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
         <v>8.5371703132912735</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="8">
         <v>256</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
         <v>2593.52</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="8">
         <f t="shared" si="0"/>
         <v>5.5451774444795623</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>7.8607713053483801</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="8">
         <v>512</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <v>1311.84</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="8">
         <f t="shared" si="0"/>
         <v>6.2383246250395077</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
         <v>7.1791860108478671</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="8">
         <v>1024</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <v>744.75</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="8">
         <f t="shared" si="0"/>
         <v>6.9314718055994531</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="8">
         <f t="shared" si="0"/>
         <v>6.6130485915933921</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="8">
         <v>1536</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="8">
         <v>479.87</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="8">
         <f t="shared" si="0"/>
         <v>7.3369369137076177</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>6.1735152338866328</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
@@ -1861,7 +1880,7 @@
         <v>4.0176434872918296</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -1880,7 +1899,7 @@
         <v>3.5804587051595158</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
@@ -1899,7 +1918,7 @@
         <v>2.997730276216664</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>2</v>
       </c>
@@ -1918,7 +1937,7 @@
         <v>1.1662709371419244</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>2</v>
       </c>
@@ -1937,113 +1956,113 @@
         <v>0.88376754016859504</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="8">
         <v>128</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="8">
         <v>32.43</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="8">
         <f t="shared" si="0"/>
         <v>4.8520302639196169</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="8">
         <f t="shared" si="0"/>
         <v>3.4790839203192268</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="8">
         <v>256</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="8">
         <v>16.079999999999998</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="8">
         <f t="shared" si="0"/>
         <v>5.5451774444795623</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="8">
         <f t="shared" si="0"/>
         <v>2.7775762637508201</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="8">
         <v>512</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="8">
         <v>6.76</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="8">
         <f t="shared" si="0"/>
         <v>6.2383246250395077</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="8">
         <f t="shared" si="0"/>
         <v>1.9110228900548727</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="8">
         <v>1024</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="8">
         <v>9</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="8">
         <f t="shared" si="0"/>
         <v>6.9314718055994531</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="8">
         <f t="shared" si="0"/>
         <v>2.1972245773362196</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="8">
         <v>1536</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="8">
         <v>6.6</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="8">
         <f t="shared" si="0"/>
         <v>7.3369369137076177</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="8">
         <f t="shared" si="0"/>
         <v>1.8870696490323797</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2053,440 +2072,142 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FEBF1-B753-4FD3-B632-9352B5345DCD}">
-  <dimension ref="A1:O29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B63D911-C6CB-40AD-B79A-ACB3F28255E6}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.99671447911551203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.99343975287850639</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.99125300383800852</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6.1213144875218464E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>'Regression - csharp'!B17</f>
+        <v>11.660021282096542</v>
+      </c>
+      <c r="C2">
+        <f>'Regression - csharp'!B18</f>
+        <v>-0.64647637599550711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
-        <v>1.7022838325144298</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1.7022838325144298</v>
-      </c>
-      <c r="E12" s="1">
-        <v>454.29984624679736</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2.2595713393633323E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="B3" s="12">
+        <f>'Regression - java'!B17</f>
+        <v>13.077553933392107</v>
+      </c>
+      <c r="C3" s="12">
+        <f>'Regression - java'!B18</f>
+        <v>-0.93917077315335684</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f>'Regression - nodejs'!B17</f>
+        <v>10.942742421629209</v>
+      </c>
+      <c r="C4">
+        <f>'Regression - nodejs'!B18</f>
+        <v>-1.3612451916850219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1">
-        <v>1.1241147316543453E-2</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3.7470491055144844E-3</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1.7135249798309733</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L16">
-        <v>128</v>
-      </c>
-      <c r="M16">
-        <f>LN(L16)</f>
-        <v>4.8520302639196169</v>
-      </c>
-      <c r="N16">
-        <f>$B$17+M16*$B$18</f>
-        <v>8.5232983408572647</v>
-      </c>
-      <c r="O16">
-        <f>EXP(N16)</f>
-        <v>5030.619119249428</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1">
-        <v>11.660021282096542</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.18945540423413776</v>
-      </c>
-      <c r="D17" s="1">
-        <v>61.5449389223363</v>
-      </c>
-      <c r="E17" s="1">
-        <v>9.451072629970514E-6</v>
-      </c>
-      <c r="F17" s="1">
-        <v>11.057089630875579</v>
-      </c>
-      <c r="G17" s="1">
-        <v>12.262952933317505</v>
-      </c>
-      <c r="H17" s="1">
-        <v>10.553429447726071</v>
-      </c>
-      <c r="I17" s="1">
-        <v>12.766613116467013</v>
-      </c>
-      <c r="L17">
-        <v>256</v>
-      </c>
-      <c r="M17">
-        <f t="shared" ref="M17:M21" si="0">LN(L17)</f>
-        <v>5.5451774444795623</v>
-      </c>
-      <c r="N17">
-        <f t="shared" ref="N17:N21" si="1">$B$17+M17*$B$18</f>
-        <v>8.0751950635373682</v>
-      </c>
-      <c r="O17">
-        <f t="shared" ref="O17:O21" si="2">EXP(N17)</f>
-        <v>3213.7541938091595</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="2">
-        <v>-0.64647637599550711</v>
-      </c>
-      <c r="C18" s="2">
-        <v>3.0330625329077279E-2</v>
-      </c>
-      <c r="D18" s="2">
-        <v>-21.314310832086438</v>
-      </c>
-      <c r="E18" s="2">
-        <v>2.2595713393633323E-4</v>
-      </c>
-      <c r="F18" s="2">
-        <v>-0.74300196251097361</v>
-      </c>
-      <c r="G18" s="2">
-        <v>-0.54995078948004061</v>
-      </c>
-      <c r="H18" s="2">
-        <v>-0.82363480785014898</v>
-      </c>
-      <c r="I18" s="2">
-        <v>-0.46931794414086525</v>
-      </c>
-      <c r="L18">
-        <v>512</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="0"/>
-        <v>6.2383246250395077</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="1"/>
-        <v>7.6270917862174707</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="2"/>
-        <v>2053.0705611771555</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L19">
-        <v>1024</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="0"/>
-        <v>6.9314718055994531</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="1"/>
-        <v>7.1789885088975733</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="2"/>
-        <v>1311.5809346253266</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L20">
-        <v>1536</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="0"/>
-        <v>7.3369369137076177</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="1"/>
-        <v>6.9168648952151806</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="2"/>
-        <v>1009.1512350682101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L21">
-        <v>3008</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="0"/>
-        <v>8.0090306850697299</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="1"/>
-        <v>6.4823721495758493</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="2"/>
-        <v>653.51935467692033</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>10</v>
-      </c>
-      <c r="B25" s="1">
-        <v>6.9560214963916254</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>30</v>
-      </c>
-      <c r="B26" s="1">
-        <v>7.1855233699201051</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>50</v>
-      </c>
-      <c r="B27" s="1">
-        <v>7.5748767087176923</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>70</v>
-      </c>
-      <c r="B28" s="1">
-        <v>8.0196456885960892</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>90</v>
-      </c>
-      <c r="B29" s="2">
-        <v>8.5853713310993491</v>
+      <c r="B5" s="12">
+        <f>'Regression - python'!B17</f>
+        <v>6.16393957920255</v>
+      </c>
+      <c r="C5" s="12">
+        <f>'Regression - python'!B18</f>
+        <v>-0.60082047670970185</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B25:B29">
-    <sortCondition ref="B25"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB3C06F-AE26-4C79-A0E9-97B6A49A70CE}">
-  <dimension ref="A1:O29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FEBF1-B753-4FD3-B632-9352B5345DCD}">
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>0.99942325123676401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99671447911551203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>0.99884683511266392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99343975287850639</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>0.99846244681688523</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99125300383800852</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>3.7182922867771841E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6.1213144875218464E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2494,12 +2215,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
@@ -2517,7 +2238,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2525,19 +2246,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>3.5926573136147706</v>
+        <v>1.7022838325144298</v>
       </c>
       <c r="D12" s="1">
-        <v>3.5926573136147706</v>
+        <v>1.7022838325144298</v>
       </c>
       <c r="E12" s="1">
-        <v>2598.5360274542436</v>
+        <v>454.29984624679736</v>
       </c>
       <c r="F12" s="1">
-        <v>1.6625560279112985E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2.2595713393633323E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2545,15 +2266,15 @@
         <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>4.1477092589720099E-3</v>
+        <v>1.1241147316543453E-2</v>
       </c>
       <c r="D13" s="1">
-        <v>1.38256975299067E-3</v>
+        <v>3.7470491055144844E-3</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -2561,14 +2282,14 @@
         <v>4</v>
       </c>
       <c r="C14" s="2">
-        <v>3.5968050228737427</v>
+        <v>1.7135249798309733</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>21</v>
@@ -2603,40 +2324,48 @@
       </c>
       <c r="N16">
         <f>$B$17+M16*$B$18</f>
-        <v>8.5206689190632332</v>
+        <v>8.5232983408572647</v>
       </c>
       <c r="O16">
         <f>EXP(N16)</f>
-        <v>5017.4088749630637</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>5030.619119249428</v>
+      </c>
+      <c r="P16">
+        <f>ROUNDUP(O16,0)</f>
+        <v>5031</v>
+      </c>
+      <c r="Q16" t="str">
+        <f>"'"&amp;L16&amp;"': "&amp;P16&amp;","</f>
+        <v>'128': 5031,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>13.077553933392107</v>
+        <v>11.660021282096542</v>
       </c>
       <c r="C17" s="1">
-        <v>0.11508158414145418</v>
+        <v>0.18945540423413776</v>
       </c>
       <c r="D17" s="1">
-        <v>113.63724292600668</v>
+        <v>61.5449389223363</v>
       </c>
       <c r="E17" s="1">
-        <v>1.5024070812606606E-6</v>
+        <v>9.451072629970514E-6</v>
       </c>
       <c r="F17" s="1">
-        <v>12.711312971134939</v>
+        <v>11.057089630875579</v>
       </c>
       <c r="G17" s="1">
-        <v>13.443794895649274</v>
+        <v>12.262952933317505</v>
       </c>
       <c r="H17" s="1">
-        <v>12.405372837201424</v>
+        <v>10.553429447726071</v>
       </c>
       <c r="I17" s="1">
-        <v>13.749735029582789</v>
+        <v>12.766613116467013</v>
       </c>
       <c r="L17">
         <v>256</v>
@@ -2647,40 +2376,48 @@
       </c>
       <c r="N17">
         <f t="shared" ref="N17:N21" si="1">$B$17+M17*$B$18</f>
-        <v>7.8696853455876807</v>
+        <v>8.0751950635373682</v>
       </c>
       <c r="O17">
         <f t="shared" ref="O17:O21" si="2">EXP(N17)</f>
-        <v>2616.7420891912279</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3213.7541938091595</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17:P21" si="3">ROUNDUP(O17,0)</f>
+        <v>3214</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" ref="Q17:Q21" si="4">"'"&amp;L17&amp;"': "&amp;P17&amp;","</f>
+        <v>'256': 3214,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="2">
-        <v>-0.93917077315335684</v>
+        <v>-0.64647637599550711</v>
       </c>
       <c r="C18" s="2">
-        <v>1.8423841879735517E-2</v>
+        <v>3.0330625329077279E-2</v>
       </c>
       <c r="D18" s="2">
-        <v>-50.97583768271241</v>
+        <v>-21.314310832086438</v>
       </c>
       <c r="E18" s="2">
-        <v>1.6625560279112985E-5</v>
+        <v>2.2595713393633323E-4</v>
       </c>
       <c r="F18" s="2">
-        <v>-0.99780366067265236</v>
+        <v>-0.74300196251097361</v>
       </c>
       <c r="G18" s="2">
-        <v>-0.88053788563406132</v>
+        <v>-0.54995078948004061</v>
       </c>
       <c r="H18" s="2">
-        <v>-1.0467827627097592</v>
+        <v>-0.82363480785014898</v>
       </c>
       <c r="I18" s="2">
-        <v>-0.83155878359695434</v>
+        <v>-0.46931794414086525</v>
       </c>
       <c r="L18">
         <v>512</v>
@@ -2691,14 +2428,22 @@
       </c>
       <c r="N18">
         <f t="shared" si="1"/>
-        <v>7.2187017721121274</v>
+        <v>7.6270917862174707</v>
       </c>
       <c r="O18">
         <f t="shared" si="2"/>
-        <v>1364.7161975403635</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2053.0705611771555</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>2054</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="4"/>
+        <v>'512': 2054,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L19">
         <v>1024</v>
       </c>
@@ -2708,14 +2453,22 @@
       </c>
       <c r="N19">
         <f t="shared" si="1"/>
-        <v>6.567718198636574</v>
+        <v>7.1789885088975733</v>
       </c>
       <c r="O19">
         <f t="shared" si="2"/>
-        <v>711.7439305623991</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1311.5809346253266</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>1312</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="4"/>
+        <v>'1024': 1312,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L20">
         <v>1536</v>
       </c>
@@ -2725,14 +2478,22 @@
       </c>
       <c r="N20">
         <f t="shared" si="1"/>
-        <v>6.1869172195679196</v>
+        <v>6.9168648952151806</v>
       </c>
       <c r="O20">
         <f t="shared" si="2"/>
-        <v>486.34449953539342</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1009.1512350682101</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>1010</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="4"/>
+        <v>'1536': 1010,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L21">
         <v>3008</v>
       </c>
@@ -2742,20 +2503,28 @@
       </c>
       <c r="N21">
         <f t="shared" si="1"/>
-        <v>5.5557063926862096</v>
+        <v>6.4823721495758493</v>
       </c>
       <c r="O21">
         <f t="shared" si="2"/>
-        <v>258.70965059395564</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>653.51935467692033</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>654</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="4"/>
+        <v>'3008': 654,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -2763,44 +2532,44 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>10</v>
       </c>
       <c r="B25" s="1">
-        <v>6.1735152338866328</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6.9560214963916254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>30</v>
       </c>
       <c r="B26" s="1">
-        <v>6.6130485915933921</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7.1855233699201051</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>50</v>
       </c>
       <c r="B27" s="1">
-        <v>7.1791860108478671</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7.5748767087176923</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>70</v>
       </c>
       <c r="B28" s="1">
-        <v>7.8607713053483801</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8.0196456885960892</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>90</v>
       </c>
       <c r="B29" s="2">
-        <v>8.5371703132912735</v>
+        <v>8.5853713310993491</v>
       </c>
     </row>
   </sheetData>
@@ -2813,60 +2582,60 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593D82EA-4FC6-4DF7-A0FE-35EF7A3ABE7D}">
-  <dimension ref="A1:O29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AB3C06F-AE26-4C79-A0E9-97B6A49A70CE}">
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="Q16" sqref="Q16:Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>0.9649816950100778</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99942325123676401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>0.93118967170452271</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99884683511266392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>0.90825289560603029</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99846244681688523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>0.43116827579502309</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3.7182922867771841E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2874,12 +2643,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
@@ -2897,7 +2666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2905,19 +2674,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>7.5474348605296617</v>
+        <v>3.5926573136147706</v>
       </c>
       <c r="D12" s="1">
-        <v>7.5474348605296617</v>
+        <v>3.5926573136147706</v>
       </c>
       <c r="E12" s="1">
-        <v>40.598106190072926</v>
+        <v>2598.5360274542436</v>
       </c>
       <c r="F12" s="1">
-        <v>7.8249589550080153E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.6625560279112985E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2925,15 +2694,15 @@
         <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>0.55771824615615928</v>
+        <v>4.1477092589720099E-3</v>
       </c>
       <c r="D13" s="1">
-        <v>0.18590608205205308</v>
+        <v>1.38256975299067E-3</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -2941,14 +2710,14 @@
         <v>4</v>
       </c>
       <c r="C14" s="2">
-        <v>8.1051531066858207</v>
+        <v>3.5968050228737427</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>21</v>
@@ -2983,40 +2752,48 @@
       </c>
       <c r="N16">
         <f>$B$17+M16*$B$18</f>
-        <v>4.3379395549584228</v>
+        <v>8.5206689190632332</v>
       </c>
       <c r="O16">
         <f>EXP(N16)</f>
-        <v>76.549650385827945</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>5017.4088749630637</v>
+      </c>
+      <c r="P16">
+        <f>ROUNDUP(O16,0)</f>
+        <v>5018</v>
+      </c>
+      <c r="Q16" t="str">
+        <f>"'"&amp;L16&amp;"': "&amp;P16&amp;","</f>
+        <v>'128': 5018,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>10.942742421629209</v>
+        <v>13.077553933392107</v>
       </c>
       <c r="C17" s="1">
-        <v>1.3344708910185816</v>
+        <v>0.11508158414145418</v>
       </c>
       <c r="D17" s="1">
-        <v>8.2000607845981399</v>
+        <v>113.63724292600668</v>
       </c>
       <c r="E17" s="1">
-        <v>3.7952755020816621E-3</v>
+        <v>1.5024070812606606E-6</v>
       </c>
       <c r="F17" s="1">
-        <v>6.6958604649984643</v>
+        <v>12.711312971134939</v>
       </c>
       <c r="G17" s="1">
-        <v>15.189624378259953</v>
+        <v>13.443794895649274</v>
       </c>
       <c r="H17" s="1">
-        <v>3.148218970710607</v>
+        <v>12.405372837201424</v>
       </c>
       <c r="I17" s="1">
-        <v>18.737265872547809</v>
+        <v>13.749735029582789</v>
       </c>
       <c r="L17">
         <v>256</v>
@@ -3027,40 +2804,48 @@
       </c>
       <c r="N17">
         <f t="shared" ref="N17:N21" si="1">$B$17+M17*$B$18</f>
-        <v>3.3943962882911674</v>
+        <v>7.8696853455876807</v>
       </c>
       <c r="O17">
         <f t="shared" ref="O17:O21" si="2">EXP(N17)</f>
-        <v>29.796659451688246</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2616.7420891912279</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17:P21" si="3">ROUNDUP(O17,0)</f>
+        <v>2617</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" ref="Q17:Q21" si="4">"'"&amp;L17&amp;"': "&amp;P17&amp;","</f>
+        <v>'256': 2617,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="2">
-        <v>-1.3612451916850219</v>
+        <v>-0.93917077315335684</v>
       </c>
       <c r="C18" s="2">
-        <v>0.21364044362663426</v>
+        <v>1.8423841879735517E-2</v>
       </c>
       <c r="D18" s="2">
-        <v>-6.3716643186904403</v>
+        <v>-50.97583768271241</v>
       </c>
       <c r="E18" s="2">
-        <v>7.8249589550080222E-3</v>
+        <v>1.6625560279112985E-5</v>
       </c>
       <c r="F18" s="2">
-        <v>-2.0411444321637768</v>
+        <v>-0.99780366067265236</v>
       </c>
       <c r="G18" s="2">
-        <v>-0.68134595120626718</v>
+        <v>-0.88053788563406132</v>
       </c>
       <c r="H18" s="2">
-        <v>-2.6090996477993942</v>
+        <v>-1.0467827627097592</v>
       </c>
       <c r="I18" s="2">
-        <v>-0.11339073557064938</v>
+        <v>-0.83155878359695434</v>
       </c>
       <c r="L18">
         <v>512</v>
@@ -3071,14 +2856,22 @@
       </c>
       <c r="N18">
         <f t="shared" si="1"/>
-        <v>2.4508530216239119</v>
+        <v>7.2187017721121274</v>
       </c>
       <c r="O18">
         <f t="shared" si="2"/>
-        <v>11.598236046865777</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1364.7161975403635</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>1365</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="4"/>
+        <v>'512': 1365,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L19">
         <v>1024</v>
       </c>
@@ -3088,14 +2881,22 @@
       </c>
       <c r="N19">
         <f t="shared" si="1"/>
-        <v>1.5073097549566565</v>
+        <v>6.567718198636574</v>
       </c>
       <c r="O19">
         <f t="shared" si="2"/>
-        <v>4.5145691454749635</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>711.7439305623991</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>712</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="4"/>
+        <v>'1024': 712,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L20">
         <v>1536</v>
       </c>
@@ -3105,14 +2906,22 @@
       </c>
       <c r="N20">
         <f t="shared" si="1"/>
-        <v>0.95537232614836931</v>
+        <v>6.1869172195679196</v>
       </c>
       <c r="O20">
         <f t="shared" si="2"/>
-        <v>2.5996383160735403</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>486.34449953539342</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>487</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="4"/>
+        <v>'1536': 487,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L21">
         <v>3008</v>
       </c>
@@ -3122,20 +2931,28 @@
       </c>
       <c r="N21">
         <f t="shared" si="1"/>
-        <v>4.0487911520243003E-2</v>
+        <v>5.5557063926862096</v>
       </c>
       <c r="O21">
         <f t="shared" si="2"/>
-        <v>1.041318721666145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>258.70965059395564</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>259</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="4"/>
+        <v>'3008': 259,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -3143,44 +2960,44 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>10</v>
       </c>
       <c r="B25" s="1">
-        <v>0.88376754016859504</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6.1735152338866328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>30</v>
       </c>
       <c r="B26" s="1">
-        <v>1.1662709371419244</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6.6130485915933921</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>50</v>
       </c>
       <c r="B27" s="1">
-        <v>2.997730276216664</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7.1791860108478671</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>70</v>
       </c>
       <c r="B28" s="1">
-        <v>3.5804587051595158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>7.8607713053483801</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>90</v>
       </c>
       <c r="B29" s="2">
-        <v>4.0176434872918296</v>
+        <v>8.5371703132912735</v>
       </c>
     </row>
   </sheetData>
@@ -3193,60 +3010,60 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3256631-899C-4BD1-82C4-798CEE30EB4D}">
-  <dimension ref="A1:O29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593D82EA-4FC6-4DF7-A0FE-35EF7A3ABE7D}">
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="Q16" sqref="Q16:Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>0.89450421183478013</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.9649816950100778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>0.80013778499016119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.93118967170452271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>0.73351704665354822</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.90825289560603029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>0.34988907685923337</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.43116827579502309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -3254,12 +3071,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
@@ -3277,7 +3094,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -3285,19 +3102,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>1.4703343627610508</v>
+        <v>7.5474348605296617</v>
       </c>
       <c r="D12" s="1">
-        <v>1.4703343627610508</v>
+        <v>7.5474348605296617</v>
       </c>
       <c r="E12" s="1">
-        <v>12.01034099843392</v>
+        <v>40.598106190072926</v>
       </c>
       <c r="F12" s="1">
-        <v>4.0475477471786175E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7.8249589550080153E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -3305,15 +3122,15 @@
         <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>0.36726709831621951</v>
+        <v>0.55771824615615928</v>
       </c>
       <c r="D13" s="1">
-        <v>0.12242236610540651</v>
+        <v>0.18590608205205308</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -3321,14 +3138,14 @@
         <v>4</v>
       </c>
       <c r="C14" s="2">
-        <v>1.8376014610772704</v>
+        <v>8.1051531066858207</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>21</v>
@@ -3363,14 +3180,450 @@
       </c>
       <c r="N16">
         <f>$B$17+M16*$B$18</f>
+        <v>4.3379395549584228</v>
+      </c>
+      <c r="O16">
+        <f>EXP(N16)</f>
+        <v>76.549650385827945</v>
+      </c>
+      <c r="P16">
+        <f>ROUNDUP(O16,0)</f>
+        <v>77</v>
+      </c>
+      <c r="Q16" t="str">
+        <f>"'"&amp;L16&amp;"': "&amp;P16&amp;","</f>
+        <v>'128': 77,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10.942742421629209</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.3344708910185816</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8.2000607845981399</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3.7952755020816621E-3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6.6958604649984643</v>
+      </c>
+      <c r="G17" s="1">
+        <v>15.189624378259953</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3.148218970710607</v>
+      </c>
+      <c r="I17" s="1">
+        <v>18.737265872547809</v>
+      </c>
+      <c r="L17">
+        <v>256</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ref="M17:M21" si="0">LN(L17)</f>
+        <v>5.5451774444795623</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ref="N17:N21" si="1">$B$17+M17*$B$18</f>
+        <v>3.3943962882911674</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ref="O17:O21" si="2">EXP(N17)</f>
+        <v>29.796659451688246</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17:P21" si="3">ROUNDUP(O17,0)</f>
+        <v>30</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" ref="Q17:Q21" si="4">"'"&amp;L17&amp;"': "&amp;P17&amp;","</f>
+        <v>'256': 30,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2">
+        <v>-1.3612451916850219</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.21364044362663426</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-6.3716643186904403</v>
+      </c>
+      <c r="E18" s="2">
+        <v>7.8249589550080222E-3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-2.0411444321637768</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-0.68134595120626718</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-2.6090996477993942</v>
+      </c>
+      <c r="I18" s="2">
+        <v>-0.11339073557064938</v>
+      </c>
+      <c r="L18">
+        <v>512</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>6.2383246250395077</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>2.4508530216239119</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>11.598236046865777</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="4"/>
+        <v>'512': 12,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>1024</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>6.9314718055994531</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>1.5073097549566565</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="2"/>
+        <v>4.5145691454749635</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="4"/>
+        <v>'1024': 5,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>1536</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>7.3369369137076177</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>0.95537232614836931</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>2.5996383160735403</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="4"/>
+        <v>'1536': 3,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>3008</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>8.0090306850697299</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>4.0487911520243003E-2</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>1.041318721666145</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="4"/>
+        <v>'3008': 2,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.88376754016859504</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.1662709371419244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>50</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2.997730276216664</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>70</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3.5804587051595158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>90</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4.0176434872918296</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B25:B29">
+    <sortCondition ref="B25"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3256631-899C-4BD1-82C4-798CEE30EB4D}">
+  <dimension ref="A1:Q29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.89450421183478013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.80013778499016119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.73351704665354822</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.34988907685923337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.4703343627610508</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.4703343627610508</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12.01034099843392</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.0475477471786175E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.36726709831621951</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.12242236610540651</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.8376014610772704</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16">
+        <v>128</v>
+      </c>
+      <c r="M16">
+        <f>LN(L16)</f>
+        <v>4.8520302639196169</v>
+      </c>
+      <c r="N16">
+        <f>$B$17+M16*$B$18</f>
         <v>3.2487404430244653</v>
       </c>
       <c r="O16">
         <f>EXP(N16)</f>
         <v>25.757875964040235</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <f>ROUNDUP(O16,0)</f>
+        <v>26</v>
+      </c>
+      <c r="Q16" t="str">
+        <f>"'"&amp;L16&amp;"': "&amp;P16&amp;","</f>
+        <v>'128': 26,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -3413,8 +3666,16 @@
         <f t="shared" ref="O17:O21" si="2">EXP(N17)</f>
         <v>16.984198699857068</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <f t="shared" ref="P17:P21" si="3">ROUNDUP(O17,0)</f>
+        <v>17</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" ref="Q17:Q21" si="4">"'"&amp;L17&amp;"': "&amp;P17&amp;","</f>
+        <v>'256': 17,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -3457,8 +3718,16 @@
         <f t="shared" si="2"/>
         <v>11.199021451882935</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="4"/>
+        <v>'512': 12,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L19">
         <v>1024</v>
       </c>
@@ -3474,8 +3743,16 @@
         <f t="shared" si="2"/>
         <v>7.3843979157397435</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="4"/>
+        <v>'1024': 8,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L20">
         <v>1536</v>
       </c>
@@ -3491,8 +3768,16 @@
         <f t="shared" si="2"/>
         <v>5.7878312032580279</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="4"/>
+        <v>'1536': 6,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L21">
         <v>3008</v>
       </c>
@@ -3508,14 +3793,22 @@
         <f t="shared" si="2"/>
         <v>3.8649546366720879</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="4"/>
+        <v>'3008': 4,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -3523,7 +3816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>10</v>
       </c>
@@ -3531,7 +3824,7 @@
         <v>1.8870696490323797</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>30</v>
       </c>
@@ -3539,7 +3832,7 @@
         <v>1.9110228900548727</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>50</v>
       </c>
@@ -3547,7 +3840,7 @@
         <v>2.1972245773362196</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>70</v>
       </c>
@@ -3555,7 +3848,7 @@
         <v>2.7775762637508201</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>90</v>
       </c>

</xml_diff>